<commit_message>
Add properly formatted revision questions
</commit_message>
<xml_diff>
--- a/docs/revision.xlsx
+++ b/docs/revision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jparsons/Desktop/quiz-app/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C87F673-5BFD-5B45-AADB-42491E3FC39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAA569C-2C31-6445-90BB-979F6725613A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="2360" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="277">
-  <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="275">
   <si>
     <t>Define the term 'bit'.</t>
   </si>
@@ -857,16 +851,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -882,7 +868,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -890,30 +876,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,19 +1186,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B140"/>
+  <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1388,18 +1356,18 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2164,15 +2132,15 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
+        <v>144</v>
+      </c>
+      <c r="B118" t="s">
         <v>232</v>
-      </c>
-      <c r="B118" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>146</v>
+        <v>233</v>
       </c>
       <c r="B119" t="s">
         <v>234</v>
@@ -2336,14 +2304,6 @@
       </c>
       <c r="B139" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>275</v>
-      </c>
-      <c r="B140" t="s">
-        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>